<commit_message>
Update sprint 7 backlog
</commit_message>
<xml_diff>
--- a/docs/process/sprint-7-backlog.xlsx
+++ b/docs/process/sprint-7-backlog.xlsx
@@ -9,14 +9,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="qVufQvxsCpbMyyokKvZeVcROiK2ABi5bwewMM1dS9is="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="+jF0LL7Vv5FOGgIuLeqmyxdXTmmUOATGwt6QIJX3NSQ="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Remaining effort at the end of the day ...</t>
   </si>
@@ -42,6 +42,9 @@
     <t>Artegiani</t>
   </si>
   <si>
+    <t>Giocatore immune agli effetti dopo aver chiamato cactus</t>
+  </si>
+  <si>
     <t>Tavolo di gioco</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
   </si>
   <si>
     <t>Aggiunta effetto speciale Jack view</t>
+  </si>
+  <si>
+    <t>Quando un giocatore chiama cactus la sua mano viene scoperta</t>
   </si>
 </sst>
 </file>
@@ -390,14 +396,12 @@
       <c r="F3" s="1"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1">
         <v>2.0</v>
@@ -407,41 +411,59 @@
       <c r="G4" s="2"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="3"/>
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D5" s="1">
         <v>2.0</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="5"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="L7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="3"/>
       <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="L8" s="1"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="3"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
@@ -459,13 +481,17 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+    <row r="13" ht="15.75" customHeight="1">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
     <row r="16" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
@@ -1448,6 +1474,7 @@
     <row r="995" ht="15.75" customHeight="1"/>
     <row r="996" ht="15.75" customHeight="1"/>
     <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>